<commit_message>
debugged max date for recent game issue
</commit_message>
<xml_diff>
--- a/THE Halo Statline.xlsx
+++ b/THE Halo Statline.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="36">
   <si>
     <t>Overall -- Cumulative</t>
   </si>
@@ -101,31 +101,31 @@
     <t>k/d spread</t>
   </si>
   <si>
-    <t>Overall -- Recent Halo Night On 3/2/21</t>
+    <t>Overall -- Recent Halo Night On 3/16/21</t>
   </si>
   <si>
     <t>Blackout -- Cumulative</t>
   </si>
   <si>
-    <t>Blackout -- Recent Halo Night On 3/2/21</t>
+    <t>Blackout -- Recent Halo Night On 3/16/21</t>
   </si>
   <si>
     <t>Construct -- Cumulative</t>
   </si>
   <si>
-    <t>Construct -- Recent Halo Night On 3/2/21</t>
+    <t>Construct -- Recent Halo Night On 3/16/21</t>
   </si>
   <si>
     <t>Guardian -- Cumulative</t>
   </si>
   <si>
-    <t>Guardian -- Recent Halo Night On 3/2/21</t>
+    <t>Guardian -- Recent Halo Night On 3/16/21</t>
   </si>
   <si>
     <t>The Pit -- Cumulative</t>
   </si>
   <si>
-    <t>The Pit -- Recent Halo Night On 3/2/21</t>
+    <t>The Pit -- Recent Halo Night On 3/16/21</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -584,7 +584,7 @@
         <v>5</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -593,49 +593,49 @@
         <v>5</v>
       </c>
       <c r="K4">
-        <v>51.9</v>
+        <v>55.3</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O4">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S4">
-        <v>14.3</v>
+        <v>14.2</v>
       </c>
       <c r="T4">
-        <v>7.6</v>
+        <v>6.9</v>
       </c>
       <c r="U4">
-        <v>13</v>
+        <v>11.4</v>
       </c>
       <c r="W4" s="1">
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y4">
-        <v>387</v>
+        <v>540</v>
       </c>
       <c r="Z4">
-        <v>206</v>
+        <v>264</v>
       </c>
       <c r="AA4">
-        <v>352</v>
+        <v>434</v>
       </c>
       <c r="AB4">
-        <v>35</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -646,67 +646,67 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K5">
-        <v>51.9</v>
+        <v>52.6</v>
       </c>
       <c r="M5" s="1">
         <v>2</v>
       </c>
       <c r="N5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O5">
-        <v>1.18</v>
+        <v>1.24</v>
       </c>
       <c r="Q5" s="1">
         <v>2</v>
       </c>
       <c r="R5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S5">
         <v>13.9</v>
       </c>
       <c r="T5">
-        <v>6.8</v>
+        <v>7.6</v>
       </c>
       <c r="U5">
-        <v>10.7</v>
+        <v>13.3</v>
       </c>
       <c r="W5" s="1">
         <v>2</v>
       </c>
       <c r="X5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Y5">
-        <v>376</v>
+        <v>527</v>
       </c>
       <c r="Z5">
-        <v>183</v>
+        <v>290</v>
       </c>
       <c r="AA5">
-        <v>288</v>
+        <v>507</v>
       </c>
       <c r="AB5">
-        <v>88</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -717,25 +717,25 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="I6" s="1">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K6">
-        <v>51.9</v>
+        <v>52.6</v>
       </c>
       <c r="M6" s="1">
         <v>3</v>
@@ -744,7 +744,7 @@
         <v>10</v>
       </c>
       <c r="O6">
-        <v>1.1</v>
+        <v>1.04</v>
       </c>
       <c r="Q6" s="1">
         <v>3</v>
@@ -753,13 +753,13 @@
         <v>4</v>
       </c>
       <c r="S6">
-        <v>12.8</v>
+        <v>13.2</v>
       </c>
       <c r="T6">
-        <v>8.1</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="U6">
-        <v>10.8</v>
+        <v>10.1</v>
       </c>
       <c r="W6" s="1">
         <v>3</v>
@@ -768,16 +768,16 @@
         <v>4</v>
       </c>
       <c r="Y6">
-        <v>345</v>
+        <v>501</v>
       </c>
       <c r="Z6">
-        <v>219</v>
+        <v>310</v>
       </c>
       <c r="AA6">
-        <v>292</v>
+        <v>385</v>
       </c>
       <c r="AB6">
-        <v>53</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -788,34 +788,34 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1">
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I7" s="1">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K7">
-        <v>51.9</v>
+        <v>50</v>
       </c>
       <c r="M7" s="1">
         <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="Q7" s="1">
         <v>4</v>
@@ -824,13 +824,13 @@
         <v>7</v>
       </c>
       <c r="S7">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="T7">
-        <v>7</v>
+        <v>7.7</v>
       </c>
       <c r="U7">
-        <v>13</v>
+        <v>12.8</v>
       </c>
       <c r="W7" s="1">
         <v>4</v>
@@ -839,16 +839,16 @@
         <v>7</v>
       </c>
       <c r="Y7">
-        <v>330</v>
+        <v>458</v>
       </c>
       <c r="Z7">
-        <v>189</v>
+        <v>293</v>
       </c>
       <c r="AA7">
-        <v>352</v>
+        <v>488</v>
       </c>
       <c r="AB7">
-        <v>-22</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -859,34 +859,34 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1">
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1">
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K8">
-        <v>48.1</v>
+        <v>50</v>
       </c>
       <c r="M8" s="1">
         <v>5</v>
       </c>
       <c r="N8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O8">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="Q8" s="1">
         <v>5</v>
@@ -901,7 +901,7 @@
         <v>7.3</v>
       </c>
       <c r="U8">
-        <v>11.3</v>
+        <v>12</v>
       </c>
       <c r="W8" s="1">
         <v>5</v>
@@ -910,16 +910,16 @@
         <v>6</v>
       </c>
       <c r="Y8">
-        <v>304</v>
+        <v>431</v>
       </c>
       <c r="Z8">
-        <v>198</v>
+        <v>278</v>
       </c>
       <c r="AA8">
-        <v>304</v>
+        <v>456</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -930,25 +930,25 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1">
         <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K9">
-        <v>48.1</v>
+        <v>50</v>
       </c>
       <c r="M9" s="1">
         <v>6</v>
@@ -969,10 +969,10 @@
         <v>10.1</v>
       </c>
       <c r="T9">
-        <v>8.5</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="U9">
-        <v>13</v>
+        <v>12.9</v>
       </c>
       <c r="W9" s="1">
         <v>6</v>
@@ -981,16 +981,16 @@
         <v>9</v>
       </c>
       <c r="Y9">
-        <v>273</v>
+        <v>383</v>
       </c>
       <c r="Z9">
-        <v>230</v>
+        <v>336</v>
       </c>
       <c r="AA9">
-        <v>352</v>
+        <v>492</v>
       </c>
       <c r="AB9">
-        <v>-79</v>
+        <v>-109</v>
       </c>
     </row>
     <row r="10" spans="1:28">
@@ -1001,34 +1001,34 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I10" s="1">
         <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K10">
-        <v>48.1</v>
+        <v>44.7</v>
       </c>
       <c r="M10" s="1">
         <v>7</v>
       </c>
       <c r="N10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O10">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="Q10" s="1">
         <v>7</v>
@@ -1037,13 +1037,13 @@
         <v>8</v>
       </c>
       <c r="S10">
-        <v>9.699999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="T10">
-        <v>6.8</v>
+        <v>7.2</v>
       </c>
       <c r="U10">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="W10" s="1">
         <v>7</v>
@@ -1052,16 +1052,16 @@
         <v>8</v>
       </c>
       <c r="Y10">
-        <v>261</v>
+        <v>372</v>
       </c>
       <c r="Z10">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="AA10">
-        <v>270</v>
+        <v>378</v>
       </c>
       <c r="AB10">
-        <v>-9</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -1072,34 +1072,34 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I11" s="1">
         <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K11">
-        <v>48.1</v>
+        <v>44.7</v>
       </c>
       <c r="M11" s="1">
         <v>8</v>
       </c>
       <c r="N11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O11">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="Q11" s="1">
         <v>8</v>
@@ -1111,10 +1111,10 @@
         <v>9.199999999999999</v>
       </c>
       <c r="T11">
-        <v>8.800000000000001</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="U11">
-        <v>12.1</v>
+        <v>11.5</v>
       </c>
       <c r="W11" s="1">
         <v>8</v>
@@ -1123,16 +1123,16 @@
         <v>11</v>
       </c>
       <c r="Y11">
-        <v>248</v>
+        <v>348</v>
       </c>
       <c r="Z11">
-        <v>237</v>
+        <v>329</v>
       </c>
       <c r="AA11">
-        <v>326</v>
+        <v>438</v>
       </c>
       <c r="AB11">
-        <v>-78</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -1221,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1230,7 +1230,7 @@
         <v>5</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
@@ -1239,49 +1239,49 @@
         <v>5</v>
       </c>
       <c r="K16">
-        <v>53.8</v>
+        <v>60</v>
       </c>
       <c r="M16" s="1">
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O16">
-        <v>1.56</v>
+        <v>1.7</v>
       </c>
       <c r="Q16" s="1">
         <v>1</v>
       </c>
       <c r="R16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16">
+        <v>15.8</v>
+      </c>
+      <c r="T16">
+        <v>7.6</v>
+      </c>
+      <c r="U16">
+        <v>13.8</v>
+      </c>
+      <c r="W16" s="1">
+        <v>1</v>
+      </c>
+      <c r="X16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y16">
+        <v>79</v>
+      </c>
+      <c r="Z16">
+        <v>38</v>
+      </c>
+      <c r="AA16">
+        <v>69</v>
+      </c>
+      <c r="AB16">
         <v>10</v>
-      </c>
-      <c r="S16">
-        <v>14.7</v>
-      </c>
-      <c r="T16">
-        <v>7.2</v>
-      </c>
-      <c r="U16">
-        <v>14.1</v>
-      </c>
-      <c r="W16" s="1">
-        <v>1</v>
-      </c>
-      <c r="X16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y16">
-        <v>191</v>
-      </c>
-      <c r="Z16">
-        <v>93</v>
-      </c>
-      <c r="AA16">
-        <v>183</v>
-      </c>
-      <c r="AB16">
-        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -1292,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -1301,7 +1301,7 @@
         <v>6</v>
       </c>
       <c r="G17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1">
         <v>2</v>
@@ -1310,49 +1310,49 @@
         <v>6</v>
       </c>
       <c r="K17">
-        <v>53.8</v>
+        <v>60</v>
       </c>
       <c r="M17" s="1">
         <v>2</v>
       </c>
       <c r="N17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O17">
-        <v>1.05</v>
+        <v>1.14</v>
       </c>
       <c r="Q17" s="1">
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S17">
-        <v>14.1</v>
+        <v>14.6</v>
       </c>
       <c r="T17">
-        <v>6.3</v>
+        <v>8.6</v>
       </c>
       <c r="U17">
-        <v>9</v>
+        <v>8.6</v>
       </c>
       <c r="W17" s="1">
         <v>2</v>
       </c>
       <c r="X17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y17">
-        <v>183</v>
+        <v>73</v>
       </c>
       <c r="Z17">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="AA17">
-        <v>117</v>
+        <v>43</v>
       </c>
       <c r="AB17">
-        <v>66</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:28">
@@ -1363,7 +1363,7 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
@@ -1372,7 +1372,7 @@
         <v>7</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1">
         <v>3</v>
@@ -1381,49 +1381,49 @@
         <v>7</v>
       </c>
       <c r="K18">
-        <v>53.8</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1">
         <v>3</v>
       </c>
       <c r="N18" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O18">
-        <v>1.04</v>
+        <v>1.02</v>
       </c>
       <c r="Q18" s="1">
         <v>3</v>
       </c>
       <c r="R18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S18">
-        <v>12.9</v>
+        <v>12.8</v>
       </c>
       <c r="T18">
         <v>8.199999999999999</v>
       </c>
       <c r="U18">
-        <v>13.2</v>
+        <v>14.2</v>
       </c>
       <c r="W18" s="1">
         <v>3</v>
       </c>
       <c r="X18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y18">
-        <v>168</v>
+        <v>64</v>
       </c>
       <c r="Z18">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="AA18">
-        <v>172</v>
+        <v>71</v>
       </c>
       <c r="AB18">
-        <v>-4</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="19" spans="1:28">
@@ -1434,67 +1434,67 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K19">
-        <v>53.8</v>
+        <v>60</v>
       </c>
       <c r="M19" s="1">
         <v>4</v>
       </c>
       <c r="N19" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O19">
-        <v>0.98</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="Q19" s="1">
         <v>4</v>
       </c>
       <c r="R19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="S19">
-        <v>11.9</v>
+        <v>12.6</v>
       </c>
       <c r="T19">
         <v>9</v>
       </c>
       <c r="U19">
-        <v>12.8</v>
+        <v>13.4</v>
       </c>
       <c r="W19" s="1">
         <v>4</v>
       </c>
       <c r="X19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y19">
-        <v>155</v>
+        <v>63</v>
       </c>
       <c r="Z19">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="AA19">
-        <v>166</v>
+        <v>67</v>
       </c>
       <c r="AB19">
-        <v>-11</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="20" spans="1:28">
@@ -1505,7 +1505,7 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -1514,7 +1514,7 @@
         <v>4</v>
       </c>
       <c r="G20">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I20" s="1">
         <v>5</v>
@@ -1523,49 +1523,49 @@
         <v>4</v>
       </c>
       <c r="K20">
-        <v>46.2</v>
+        <v>40</v>
       </c>
       <c r="M20" s="1">
         <v>5</v>
       </c>
       <c r="N20" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O20">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="Q20" s="1">
         <v>5</v>
       </c>
       <c r="R20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S20">
-        <v>11.5</v>
+        <v>11.6</v>
       </c>
       <c r="T20">
-        <v>7.5</v>
+        <v>10.2</v>
       </c>
       <c r="U20">
-        <v>11</v>
+        <v>11.4</v>
       </c>
       <c r="W20" s="1">
         <v>5</v>
       </c>
       <c r="X20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y20">
-        <v>150</v>
+        <v>58</v>
       </c>
       <c r="Z20">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="AA20">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="AB20">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:28">
@@ -1576,7 +1576,7 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
@@ -1585,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="G21">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I21" s="1">
         <v>6</v>
@@ -1594,13 +1594,13 @@
         <v>8</v>
       </c>
       <c r="K21">
-        <v>46.2</v>
+        <v>40</v>
       </c>
       <c r="M21" s="1">
         <v>6</v>
       </c>
       <c r="N21" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O21">
         <v>0.9</v>
@@ -1609,34 +1609,34 @@
         <v>6</v>
       </c>
       <c r="R21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S21">
-        <v>10.3</v>
+        <v>11</v>
       </c>
       <c r="T21">
-        <v>8.5</v>
+        <v>9.4</v>
       </c>
       <c r="U21">
-        <v>12.8</v>
+        <v>12.4</v>
       </c>
       <c r="W21" s="1">
         <v>6</v>
       </c>
       <c r="X21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y21">
-        <v>134</v>
+        <v>55</v>
       </c>
       <c r="Z21">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="AA21">
-        <v>167</v>
+        <v>62</v>
       </c>
       <c r="AB21">
-        <v>-33</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="22" spans="1:28">
@@ -1647,67 +1647,67 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1">
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I22" s="1">
         <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K22">
-        <v>46.2</v>
+        <v>40</v>
       </c>
       <c r="M22" s="1">
         <v>7</v>
       </c>
       <c r="N22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O22">
-        <v>0.8</v>
+        <v>0.89</v>
       </c>
       <c r="Q22" s="1">
         <v>7</v>
       </c>
       <c r="R22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S22">
-        <v>9.300000000000001</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="T22">
-        <v>8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="U22">
-        <v>11.9</v>
+        <v>13.8</v>
       </c>
       <c r="W22" s="1">
         <v>7</v>
       </c>
       <c r="X22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y22">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="Z22">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="AA22">
-        <v>155</v>
+        <v>69</v>
       </c>
       <c r="AB22">
-        <v>-34</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="23" spans="1:28">
@@ -1718,67 +1718,67 @@
         <v>11</v>
       </c>
       <c r="C23">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
       </c>
       <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>40</v>
+      </c>
+      <c r="M23" s="1">
+        <v>8</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23">
+        <v>0.71</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>8</v>
+      </c>
+      <c r="R23" t="s">
         <v>11</v>
       </c>
-      <c r="G23">
-        <v>6</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="S23">
+        <v>7.8</v>
+      </c>
+      <c r="T23">
+        <v>7.4</v>
+      </c>
+      <c r="U23">
+        <v>8.6</v>
+      </c>
+      <c r="W23" s="1">
+        <v>8</v>
+      </c>
+      <c r="X23" t="s">
         <v>11</v>
       </c>
-      <c r="K23">
-        <v>46.2</v>
-      </c>
-      <c r="M23" s="1">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23">
-        <v>0.78</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>8</v>
-      </c>
-      <c r="R23" t="s">
-        <v>8</v>
-      </c>
-      <c r="S23">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="T23">
-        <v>6.6</v>
-      </c>
-      <c r="U23">
-        <v>10.3</v>
-      </c>
-      <c r="W23" s="1">
-        <v>8</v>
-      </c>
-      <c r="X23" t="s">
-        <v>8</v>
-      </c>
       <c r="Y23">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="Z23">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="AA23">
-        <v>134</v>
+        <v>43</v>
       </c>
       <c r="AB23">
-        <v>-14</v>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +1788,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2516,574 +2516,6 @@
       </c>
       <c r="AB15" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16">
-        <v>75</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
-        <v>5</v>
-      </c>
-      <c r="O16">
-        <v>2.41</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16">
-        <v>17</v>
-      </c>
-      <c r="T16">
-        <v>7.2</v>
-      </c>
-      <c r="U16">
-        <v>16.2</v>
-      </c>
-      <c r="W16" s="1">
-        <v>1</v>
-      </c>
-      <c r="X16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y16">
-        <v>68</v>
-      </c>
-      <c r="Z16">
-        <v>29</v>
-      </c>
-      <c r="AA16">
-        <v>65</v>
-      </c>
-      <c r="AB16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="I17" s="1">
-        <v>2</v>
-      </c>
-      <c r="J17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17">
-        <v>75</v>
-      </c>
-      <c r="M17" s="1">
-        <v>2</v>
-      </c>
-      <c r="N17" t="s">
-        <v>11</v>
-      </c>
-      <c r="O17">
-        <v>1.16</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>5</v>
-      </c>
-      <c r="S17">
-        <v>16.2</v>
-      </c>
-      <c r="T17">
-        <v>4.2</v>
-      </c>
-      <c r="U17">
-        <v>6.8</v>
-      </c>
-      <c r="W17" s="1">
-        <v>2</v>
-      </c>
-      <c r="X17" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y17">
-        <v>65</v>
-      </c>
-      <c r="Z17">
-        <v>17</v>
-      </c>
-      <c r="AA17">
-        <v>27</v>
-      </c>
-      <c r="AB17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="E18" s="1">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>3</v>
-      </c>
-      <c r="I18" s="1">
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18">
-        <v>75</v>
-      </c>
-      <c r="M18" s="1">
-        <v>3</v>
-      </c>
-      <c r="N18" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18">
-        <v>1.11</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>3</v>
-      </c>
-      <c r="R18" t="s">
-        <v>7</v>
-      </c>
-      <c r="S18">
-        <v>11.5</v>
-      </c>
-      <c r="T18">
-        <v>8.5</v>
-      </c>
-      <c r="U18">
-        <v>14.5</v>
-      </c>
-      <c r="W18" s="1">
-        <v>3</v>
-      </c>
-      <c r="X18" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y18">
-        <v>46</v>
-      </c>
-      <c r="Z18">
-        <v>34</v>
-      </c>
-      <c r="AA18">
-        <v>58</v>
-      </c>
-      <c r="AB18">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19">
-        <v>3</v>
-      </c>
-      <c r="I19" s="1">
-        <v>4</v>
-      </c>
-      <c r="J19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19">
-        <v>75</v>
-      </c>
-      <c r="M19" s="1">
-        <v>4</v>
-      </c>
-      <c r="N19" t="s">
-        <v>10</v>
-      </c>
-      <c r="O19">
-        <v>1.05</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>4</v>
-      </c>
-      <c r="R19" t="s">
-        <v>11</v>
-      </c>
-      <c r="S19">
-        <v>11</v>
-      </c>
-      <c r="T19">
-        <v>6.5</v>
-      </c>
-      <c r="U19">
-        <v>9.5</v>
-      </c>
-      <c r="W19" s="1">
-        <v>4</v>
-      </c>
-      <c r="X19" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y19">
-        <v>44</v>
-      </c>
-      <c r="Z19">
-        <v>26</v>
-      </c>
-      <c r="AA19">
-        <v>38</v>
-      </c>
-      <c r="AB19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1">
-        <v>5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20">
-        <v>25</v>
-      </c>
-      <c r="M20" s="1">
-        <v>5</v>
-      </c>
-      <c r="N20" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20">
-        <v>0.96</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>5</v>
-      </c>
-      <c r="R20" t="s">
-        <v>6</v>
-      </c>
-      <c r="S20">
-        <v>10.8</v>
-      </c>
-      <c r="T20">
-        <v>5</v>
-      </c>
-      <c r="U20">
-        <v>11.2</v>
-      </c>
-      <c r="W20" s="1">
-        <v>5</v>
-      </c>
-      <c r="X20" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y20">
-        <v>43</v>
-      </c>
-      <c r="Z20">
-        <v>20</v>
-      </c>
-      <c r="AA20">
-        <v>45</v>
-      </c>
-      <c r="AB20">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1">
-        <v>6</v>
-      </c>
-      <c r="J21" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21">
-        <v>25</v>
-      </c>
-      <c r="M21" s="1">
-        <v>6</v>
-      </c>
-      <c r="N21" t="s">
-        <v>7</v>
-      </c>
-      <c r="O21">
-        <v>0.79</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>6</v>
-      </c>
-      <c r="R21" t="s">
-        <v>9</v>
-      </c>
-      <c r="S21">
-        <v>10.8</v>
-      </c>
-      <c r="T21">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="U21">
-        <v>15.2</v>
-      </c>
-      <c r="W21" s="1">
-        <v>6</v>
-      </c>
-      <c r="X21" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y21">
-        <v>43</v>
-      </c>
-      <c r="Z21">
-        <v>33</v>
-      </c>
-      <c r="AA21">
-        <v>61</v>
-      </c>
-      <c r="AB21">
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28">
-      <c r="A22" s="1">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1">
-        <v>7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>7</v>
-      </c>
-      <c r="J22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22">
-        <v>25</v>
-      </c>
-      <c r="M22" s="1">
-        <v>7</v>
-      </c>
-      <c r="N22" t="s">
-        <v>9</v>
-      </c>
-      <c r="O22">
-        <v>0.7</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>7</v>
-      </c>
-      <c r="R22" t="s">
-        <v>8</v>
-      </c>
-      <c r="S22">
-        <v>10</v>
-      </c>
-      <c r="T22">
-        <v>7.8</v>
-      </c>
-      <c r="U22">
-        <v>9</v>
-      </c>
-      <c r="W22" s="1">
-        <v>7</v>
-      </c>
-      <c r="X22" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y22">
-        <v>40</v>
-      </c>
-      <c r="Z22">
-        <v>31</v>
-      </c>
-      <c r="AA22">
-        <v>36</v>
-      </c>
-      <c r="AB22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28">
-      <c r="A23" s="1">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>4</v>
-      </c>
-      <c r="E23" s="1">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8</v>
-      </c>
-      <c r="J23" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23">
-        <v>25</v>
-      </c>
-      <c r="M23" s="1">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>4</v>
-      </c>
-      <c r="O23">
-        <v>0.59</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>8</v>
-      </c>
-      <c r="R23" t="s">
-        <v>4</v>
-      </c>
-      <c r="S23">
-        <v>8.5</v>
-      </c>
-      <c r="T23">
-        <v>10.2</v>
-      </c>
-      <c r="U23">
-        <v>14.5</v>
-      </c>
-      <c r="W23" s="1">
-        <v>8</v>
-      </c>
-      <c r="X23" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y23">
-        <v>34</v>
-      </c>
-      <c r="Z23">
-        <v>41</v>
-      </c>
-      <c r="AA23">
-        <v>58</v>
-      </c>
-      <c r="AB23">
-        <v>-24</v>
       </c>
     </row>
   </sheetData>
@@ -3922,7 +3354,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -3931,7 +3363,7 @@
         <v>5</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1">
         <v>1</v>
@@ -3940,7 +3372,7 @@
         <v>5</v>
       </c>
       <c r="K4">
-        <v>58.3</v>
+        <v>60.9</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -3949,40 +3381,40 @@
         <v>4</v>
       </c>
       <c r="O4">
-        <v>1.29</v>
+        <v>1.46</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
       <c r="R4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S4">
-        <v>14.2</v>
+        <v>14.5</v>
       </c>
       <c r="T4">
         <v>7.5</v>
       </c>
       <c r="U4">
-        <v>12.4</v>
+        <v>12.7</v>
       </c>
       <c r="W4" s="1">
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Y4">
-        <v>171</v>
+        <v>333</v>
       </c>
       <c r="Z4">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="AA4">
-        <v>149</v>
+        <v>292</v>
       </c>
       <c r="AB4">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -3993,25 +3425,25 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K5">
-        <v>58.3</v>
+        <v>56.5</v>
       </c>
       <c r="M5" s="1">
         <v>2</v>
@@ -4020,40 +3452,40 @@
         <v>5</v>
       </c>
       <c r="O5">
-        <v>1.16</v>
+        <v>1.14</v>
       </c>
       <c r="Q5" s="1">
         <v>2</v>
       </c>
       <c r="R5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S5">
-        <v>14.1</v>
+        <v>13.5</v>
       </c>
       <c r="T5">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
       <c r="U5">
-        <v>12.2</v>
+        <v>13.2</v>
       </c>
       <c r="W5" s="1">
         <v>2</v>
       </c>
       <c r="X5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Y5">
-        <v>169</v>
+        <v>311</v>
       </c>
       <c r="Z5">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="AA5">
-        <v>146</v>
+        <v>304</v>
       </c>
       <c r="AB5">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -4064,25 +3496,25 @@
         <v>6</v>
       </c>
       <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6">
         <v>12</v>
       </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>7</v>
-      </c>
       <c r="I6" s="1">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K6">
-        <v>58.3</v>
+        <v>52.2</v>
       </c>
       <c r="M6" s="1">
         <v>3</v>
@@ -4091,40 +3523,40 @@
         <v>10</v>
       </c>
       <c r="O6">
-        <v>1.15</v>
+        <v>1.02</v>
       </c>
       <c r="Q6" s="1">
         <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="S6">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="T6">
-        <v>7</v>
+        <v>8.6</v>
       </c>
       <c r="U6">
-        <v>12.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="W6" s="1">
         <v>3</v>
       </c>
       <c r="X6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Y6">
-        <v>160</v>
+        <v>308</v>
       </c>
       <c r="Z6">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="AA6">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="AB6">
-        <v>7</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:28">
@@ -4135,25 +3567,25 @@
         <v>7</v>
       </c>
       <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7">
         <v>12</v>
       </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
       <c r="I7" s="1">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K7">
-        <v>58.3</v>
+        <v>52.2</v>
       </c>
       <c r="M7" s="1">
         <v>4</v>
@@ -4162,40 +3594,40 @@
         <v>7</v>
       </c>
       <c r="O7">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
         <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S7">
-        <v>12.7</v>
+        <v>12.5</v>
       </c>
       <c r="T7">
-        <v>8.9</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="U7">
-        <v>9.800000000000001</v>
+        <v>12.6</v>
       </c>
       <c r="W7" s="1">
         <v>4</v>
       </c>
       <c r="X7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y7">
-        <v>152</v>
+        <v>288</v>
       </c>
       <c r="Z7">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="AA7">
-        <v>118</v>
+        <v>289</v>
       </c>
       <c r="AB7">
-        <v>34</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -4206,34 +3638,34 @@
         <v>8</v>
       </c>
       <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8">
         <v>12</v>
       </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
       <c r="I8" s="1">
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K8">
-        <v>41.7</v>
+        <v>52.2</v>
       </c>
       <c r="M8" s="1">
         <v>5</v>
       </c>
       <c r="N8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O8">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="Q8" s="1">
         <v>5</v>
@@ -4245,10 +3677,10 @@
         <v>11.5</v>
       </c>
       <c r="T8">
-        <v>7.9</v>
+        <v>7.6</v>
       </c>
       <c r="U8">
-        <v>11.8</v>
+        <v>12.8</v>
       </c>
       <c r="W8" s="1">
         <v>5</v>
@@ -4257,16 +3689,16 @@
         <v>6</v>
       </c>
       <c r="Y8">
-        <v>138</v>
+        <v>265</v>
       </c>
       <c r="Z8">
-        <v>95</v>
+        <v>175</v>
       </c>
       <c r="AA8">
-        <v>142</v>
+        <v>294</v>
       </c>
       <c r="AB8">
-        <v>-4</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="9" spans="1:28">
@@ -4277,67 +3709,67 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E9" s="1">
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I9" s="1">
         <v>6</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K9">
-        <v>41.7</v>
+        <v>47.8</v>
       </c>
       <c r="M9" s="1">
         <v>6</v>
       </c>
       <c r="N9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O9">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="Q9" s="1">
         <v>6</v>
       </c>
       <c r="R9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S9">
-        <v>9.4</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="T9">
-        <v>9</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="U9">
-        <v>12</v>
+        <v>12.6</v>
       </c>
       <c r="W9" s="1">
         <v>6</v>
       </c>
       <c r="X9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y9">
-        <v>113</v>
+        <v>222</v>
       </c>
       <c r="Z9">
-        <v>108</v>
+        <v>215</v>
       </c>
       <c r="AA9">
-        <v>144</v>
+        <v>289</v>
       </c>
       <c r="AB9">
-        <v>-31</v>
+        <v>-67</v>
       </c>
     </row>
     <row r="10" spans="1:28">
@@ -4348,25 +3780,25 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1">
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I10" s="1">
         <v>7</v>
       </c>
       <c r="J10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K10">
-        <v>41.7</v>
+        <v>39.1</v>
       </c>
       <c r="M10" s="1">
         <v>7</v>
@@ -4375,40 +3807,40 @@
         <v>11</v>
       </c>
       <c r="O10">
-        <v>0.78</v>
+        <v>0.83</v>
       </c>
       <c r="Q10" s="1">
         <v>7</v>
       </c>
       <c r="R10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S10">
-        <v>9.300000000000001</v>
+        <v>9.6</v>
       </c>
       <c r="T10">
-        <v>9.1</v>
+        <v>7.3</v>
       </c>
       <c r="U10">
-        <v>12.4</v>
+        <v>10.1</v>
       </c>
       <c r="W10" s="1">
         <v>7</v>
       </c>
       <c r="X10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y10">
-        <v>112</v>
+        <v>221</v>
       </c>
       <c r="Z10">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="AA10">
-        <v>149</v>
+        <v>232</v>
       </c>
       <c r="AB10">
-        <v>-37</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -4419,67 +3851,67 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
       <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1">
+        <v>8</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>39.1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>8</v>
+      </c>
+      <c r="N11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>0.77</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>8</v>
+      </c>
+      <c r="R11" t="s">
         <v>11</v>
       </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="I11" s="1">
-        <v>8</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="S11">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="T11">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="U11">
+        <v>11.1</v>
+      </c>
+      <c r="W11" s="1">
+        <v>8</v>
+      </c>
+      <c r="X11" t="s">
         <v>11</v>
       </c>
-      <c r="K11">
-        <v>41.7</v>
-      </c>
-      <c r="M11" s="1">
-        <v>8</v>
-      </c>
-      <c r="N11" t="s">
-        <v>9</v>
-      </c>
-      <c r="O11">
-        <v>0.75</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>8</v>
-      </c>
-      <c r="R11" t="s">
-        <v>8</v>
-      </c>
-      <c r="S11">
-        <v>9.199999999999999</v>
-      </c>
-      <c r="T11">
-        <v>6.7</v>
-      </c>
-      <c r="U11">
-        <v>10.3</v>
-      </c>
-      <c r="W11" s="1">
-        <v>8</v>
-      </c>
-      <c r="X11" t="s">
-        <v>8</v>
-      </c>
       <c r="Y11">
-        <v>110</v>
+        <v>213</v>
       </c>
       <c r="Z11">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="AA11">
-        <v>124</v>
+        <v>256</v>
       </c>
       <c r="AB11">
-        <v>-14</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -4568,7 +4000,7 @@
         <v>4</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -4577,7 +4009,7 @@
         <v>5</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="1">
         <v>1</v>
@@ -4586,49 +4018,49 @@
         <v>5</v>
       </c>
       <c r="K16">
-        <v>66.7</v>
+        <v>60</v>
       </c>
       <c r="M16" s="1">
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O16">
-        <v>1.12</v>
+        <v>1.7</v>
       </c>
       <c r="Q16" s="1">
         <v>1</v>
       </c>
       <c r="R16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S16">
+        <v>15.8</v>
+      </c>
+      <c r="T16">
+        <v>7.6</v>
+      </c>
+      <c r="U16">
+        <v>13.8</v>
+      </c>
+      <c r="W16" s="1">
+        <v>1</v>
+      </c>
+      <c r="X16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y16">
+        <v>79</v>
+      </c>
+      <c r="Z16">
+        <v>38</v>
+      </c>
+      <c r="AA16">
+        <v>69</v>
+      </c>
+      <c r="AB16">
         <v>10</v>
-      </c>
-      <c r="S16">
-        <v>14.5</v>
-      </c>
-      <c r="T16">
-        <v>8</v>
-      </c>
-      <c r="U16">
-        <v>13.2</v>
-      </c>
-      <c r="W16" s="1">
-        <v>1</v>
-      </c>
-      <c r="X16" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y16">
-        <v>87</v>
-      </c>
-      <c r="Z16">
-        <v>48</v>
-      </c>
-      <c r="AA16">
-        <v>79</v>
-      </c>
-      <c r="AB16">
-        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -4639,7 +4071,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -4648,7 +4080,7 @@
         <v>6</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I17" s="1">
         <v>2</v>
@@ -4657,49 +4089,49 @@
         <v>6</v>
       </c>
       <c r="K17">
-        <v>66.7</v>
+        <v>60</v>
       </c>
       <c r="M17" s="1">
         <v>2</v>
       </c>
       <c r="N17" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O17">
-        <v>1.1</v>
+        <v>1.14</v>
       </c>
       <c r="Q17" s="1">
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="S17">
-        <v>14</v>
+        <v>14.6</v>
       </c>
       <c r="T17">
-        <v>7.8</v>
+        <v>8.6</v>
       </c>
       <c r="U17">
-        <v>12.8</v>
+        <v>8.6</v>
       </c>
       <c r="W17" s="1">
         <v>2</v>
       </c>
       <c r="X17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Y17">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="Z17">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AA17">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="AB17">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:28">
@@ -4710,7 +4142,7 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
@@ -4719,7 +4151,7 @@
         <v>7</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1">
         <v>3</v>
@@ -4728,7 +4160,7 @@
         <v>7</v>
       </c>
       <c r="K18">
-        <v>66.7</v>
+        <v>60</v>
       </c>
       <c r="M18" s="1">
         <v>3</v>
@@ -4737,40 +4169,40 @@
         <v>7</v>
       </c>
       <c r="O18">
-        <v>1.09</v>
+        <v>1.02</v>
       </c>
       <c r="Q18" s="1">
         <v>3</v>
       </c>
       <c r="R18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S18">
-        <v>12.5</v>
+        <v>12.8</v>
       </c>
       <c r="T18">
         <v>8.199999999999999</v>
       </c>
       <c r="U18">
-        <v>11.2</v>
+        <v>14.2</v>
       </c>
       <c r="W18" s="1">
         <v>3</v>
       </c>
       <c r="X18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Y18">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="Z18">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AA18">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AB18">
-        <v>8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="19" spans="1:28">
@@ -4781,67 +4213,67 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K19">
-        <v>66.7</v>
+        <v>60</v>
       </c>
       <c r="M19" s="1">
         <v>4</v>
       </c>
       <c r="N19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O19">
-        <v>1.04</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="Q19" s="1">
         <v>4</v>
       </c>
       <c r="R19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="S19">
-        <v>12.2</v>
+        <v>12.6</v>
       </c>
       <c r="T19">
+        <v>9</v>
+      </c>
+      <c r="U19">
+        <v>13.4</v>
+      </c>
+      <c r="W19" s="1">
+        <v>4</v>
+      </c>
+      <c r="X19" t="s">
         <v>10</v>
       </c>
-      <c r="U19">
-        <v>11.7</v>
-      </c>
-      <c r="W19" s="1">
-        <v>4</v>
-      </c>
-      <c r="X19" t="s">
-        <v>4</v>
-      </c>
       <c r="Y19">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="Z19">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="AA19">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AB19">
-        <v>3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="20" spans="1:28">
@@ -4852,7 +4284,7 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -4870,49 +4302,49 @@
         <v>4</v>
       </c>
       <c r="K20">
-        <v>33.3</v>
+        <v>40</v>
       </c>
       <c r="M20" s="1">
         <v>5</v>
       </c>
       <c r="N20" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="O20">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="Q20" s="1">
         <v>5</v>
       </c>
       <c r="R20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S20">
-        <v>11.2</v>
+        <v>11.6</v>
       </c>
       <c r="T20">
-        <v>8.5</v>
+        <v>10.2</v>
       </c>
       <c r="U20">
-        <v>12</v>
+        <v>11.4</v>
       </c>
       <c r="W20" s="1">
         <v>5</v>
       </c>
       <c r="X20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y20">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="Z20">
         <v>51</v>
       </c>
       <c r="AA20">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="AB20">
-        <v>-5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:28">
@@ -4923,7 +4355,7 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
@@ -4941,13 +4373,13 @@
         <v>8</v>
       </c>
       <c r="K21">
-        <v>33.3</v>
+        <v>40</v>
       </c>
       <c r="M21" s="1">
         <v>6</v>
       </c>
       <c r="N21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O21">
         <v>0.9</v>
@@ -4956,31 +4388,31 @@
         <v>6</v>
       </c>
       <c r="R21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S21">
-        <v>10.3</v>
+        <v>11</v>
       </c>
       <c r="T21">
-        <v>9</v>
+        <v>9.4</v>
       </c>
       <c r="U21">
-        <v>11.5</v>
+        <v>12.4</v>
       </c>
       <c r="W21" s="1">
         <v>6</v>
       </c>
       <c r="X21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y21">
+        <v>55</v>
+      </c>
+      <c r="Z21">
+        <v>47</v>
+      </c>
+      <c r="AA21">
         <v>62</v>
-      </c>
-      <c r="Z21">
-        <v>54</v>
-      </c>
-      <c r="AA21">
-        <v>69</v>
       </c>
       <c r="AB21">
         <v>-7</v>
@@ -4994,13 +4426,13 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1">
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -5009,10 +4441,10 @@
         <v>7</v>
       </c>
       <c r="J22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K22">
-        <v>33.3</v>
+        <v>40</v>
       </c>
       <c r="M22" s="1">
         <v>7</v>
@@ -5021,40 +4453,40 @@
         <v>8</v>
       </c>
       <c r="O22">
-        <v>0.87</v>
+        <v>0.89</v>
       </c>
       <c r="Q22" s="1">
         <v>7</v>
       </c>
       <c r="R22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="S22">
-        <v>10</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="T22">
-        <v>9.199999999999999</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="U22">
-        <v>12</v>
+        <v>13.8</v>
       </c>
       <c r="W22" s="1">
         <v>7</v>
       </c>
       <c r="X22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y22">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="Z22">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AA22">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="AB22">
-        <v>-12</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="23" spans="1:28">
@@ -5065,67 +4497,67 @@
         <v>11</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
       </c>
       <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>40</v>
+      </c>
+      <c r="M23" s="1">
+        <v>8</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23">
+        <v>0.71</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>8</v>
+      </c>
+      <c r="R23" t="s">
         <v>11</v>
       </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="S23">
+        <v>7.8</v>
+      </c>
+      <c r="T23">
+        <v>7.4</v>
+      </c>
+      <c r="U23">
+        <v>8.6</v>
+      </c>
+      <c r="W23" s="1">
+        <v>8</v>
+      </c>
+      <c r="X23" t="s">
         <v>11</v>
       </c>
-      <c r="K23">
-        <v>33.3</v>
-      </c>
-      <c r="M23" s="1">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23">
-        <v>0.83</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>8</v>
-      </c>
-      <c r="R23" t="s">
-        <v>8</v>
-      </c>
-      <c r="S23">
-        <v>9.800000000000001</v>
-      </c>
-      <c r="T23">
-        <v>6.3</v>
-      </c>
-      <c r="U23">
-        <v>11.3</v>
-      </c>
-      <c r="W23" s="1">
-        <v>8</v>
-      </c>
-      <c r="X23" t="s">
-        <v>8</v>
-      </c>
       <c r="Y23">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="Z23">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AA23">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="AB23">
-        <v>-9</v>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>
@@ -5135,7 +4567,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5865,574 +5297,6 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16">
-        <v>66.7</v>
-      </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-      <c r="N16" t="s">
-        <v>5</v>
-      </c>
-      <c r="O16">
-        <v>1.87</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
-        <v>4</v>
-      </c>
-      <c r="S16">
-        <v>16</v>
-      </c>
-      <c r="T16">
-        <v>5.3</v>
-      </c>
-      <c r="U16">
-        <v>12.7</v>
-      </c>
-      <c r="W16" s="1">
-        <v>1</v>
-      </c>
-      <c r="X16" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y16">
-        <v>48</v>
-      </c>
-      <c r="Z16">
-        <v>16</v>
-      </c>
-      <c r="AA16">
-        <v>38</v>
-      </c>
-      <c r="AB16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28">
-      <c r="A17" s="1">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1">
-        <v>2</v>
-      </c>
-      <c r="J17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17">
-        <v>66.7</v>
-      </c>
-      <c r="M17" s="1">
-        <v>2</v>
-      </c>
-      <c r="N17" t="s">
-        <v>6</v>
-      </c>
-      <c r="O17">
-        <v>1.54</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>5</v>
-      </c>
-      <c r="S17">
-        <v>14.3</v>
-      </c>
-      <c r="T17">
-        <v>5.3</v>
-      </c>
-      <c r="U17">
-        <v>7.7</v>
-      </c>
-      <c r="W17" s="1">
-        <v>2</v>
-      </c>
-      <c r="X17" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y17">
-        <v>43</v>
-      </c>
-      <c r="Z17">
-        <v>16</v>
-      </c>
-      <c r="AA17">
-        <v>23</v>
-      </c>
-      <c r="AB17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="E18" s="1">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="I18" s="1">
-        <v>3</v>
-      </c>
-      <c r="J18" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18">
-        <v>66.7</v>
-      </c>
-      <c r="M18" s="1">
-        <v>3</v>
-      </c>
-      <c r="N18" t="s">
-        <v>4</v>
-      </c>
-      <c r="O18">
-        <v>1.26</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>3</v>
-      </c>
-      <c r="R18" t="s">
-        <v>6</v>
-      </c>
-      <c r="S18">
-        <v>13.3</v>
-      </c>
-      <c r="T18">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="U18">
-        <v>8.699999999999999</v>
-      </c>
-      <c r="W18" s="1">
-        <v>3</v>
-      </c>
-      <c r="X18" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y18">
-        <v>40</v>
-      </c>
-      <c r="Z18">
-        <v>26</v>
-      </c>
-      <c r="AA18">
-        <v>26</v>
-      </c>
-      <c r="AB18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="I19" s="1">
-        <v>4</v>
-      </c>
-      <c r="J19" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19">
-        <v>66.7</v>
-      </c>
-      <c r="M19" s="1">
-        <v>4</v>
-      </c>
-      <c r="N19" t="s">
-        <v>7</v>
-      </c>
-      <c r="O19">
-        <v>1.03</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>4</v>
-      </c>
-      <c r="R19" t="s">
-        <v>7</v>
-      </c>
-      <c r="S19">
-        <v>12.7</v>
-      </c>
-      <c r="T19">
-        <v>8.300000000000001</v>
-      </c>
-      <c r="U19">
-        <v>12.3</v>
-      </c>
-      <c r="W19" s="1">
-        <v>4</v>
-      </c>
-      <c r="X19" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y19">
-        <v>38</v>
-      </c>
-      <c r="Z19">
-        <v>25</v>
-      </c>
-      <c r="AA19">
-        <v>37</v>
-      </c>
-      <c r="AB19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1">
-        <v>5</v>
-      </c>
-      <c r="J20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20">
-        <v>33.3</v>
-      </c>
-      <c r="M20" s="1">
-        <v>5</v>
-      </c>
-      <c r="N20" t="s">
-        <v>10</v>
-      </c>
-      <c r="O20">
-        <v>0.92</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>5</v>
-      </c>
-      <c r="R20" t="s">
-        <v>10</v>
-      </c>
-      <c r="S20">
-        <v>12</v>
-      </c>
-      <c r="T20">
-        <v>5.3</v>
-      </c>
-      <c r="U20">
-        <v>13</v>
-      </c>
-      <c r="W20" s="1">
-        <v>5</v>
-      </c>
-      <c r="X20" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y20">
-        <v>36</v>
-      </c>
-      <c r="Z20">
-        <v>16</v>
-      </c>
-      <c r="AA20">
-        <v>39</v>
-      </c>
-      <c r="AB20">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28">
-      <c r="A21" s="1">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1">
-        <v>6</v>
-      </c>
-      <c r="J21" t="s">
-        <v>8</v>
-      </c>
-      <c r="K21">
-        <v>33.3</v>
-      </c>
-      <c r="M21" s="1">
-        <v>6</v>
-      </c>
-      <c r="N21" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21">
-        <v>0.78</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>6</v>
-      </c>
-      <c r="R21" t="s">
-        <v>9</v>
-      </c>
-      <c r="S21">
-        <v>9.699999999999999</v>
-      </c>
-      <c r="T21">
-        <v>8</v>
-      </c>
-      <c r="U21">
-        <v>12.3</v>
-      </c>
-      <c r="W21" s="1">
-        <v>6</v>
-      </c>
-      <c r="X21" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y21">
-        <v>29</v>
-      </c>
-      <c r="Z21">
-        <v>24</v>
-      </c>
-      <c r="AA21">
-        <v>37</v>
-      </c>
-      <c r="AB21">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28">
-      <c r="A22" s="1">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="E22" s="1">
-        <v>7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>7</v>
-      </c>
-      <c r="J22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22">
-        <v>33.3</v>
-      </c>
-      <c r="M22" s="1">
-        <v>7</v>
-      </c>
-      <c r="N22" t="s">
-        <v>8</v>
-      </c>
-      <c r="O22">
-        <v>0.7</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>7</v>
-      </c>
-      <c r="R22" t="s">
-        <v>8</v>
-      </c>
-      <c r="S22">
-        <v>7</v>
-      </c>
-      <c r="T22">
-        <v>5.7</v>
-      </c>
-      <c r="U22">
-        <v>10</v>
-      </c>
-      <c r="W22" s="1">
-        <v>7</v>
-      </c>
-      <c r="X22" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y22">
-        <v>21</v>
-      </c>
-      <c r="Z22">
-        <v>17</v>
-      </c>
-      <c r="AA22">
-        <v>30</v>
-      </c>
-      <c r="AB22">
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28">
-      <c r="A23" s="1">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="E23" s="1">
-        <v>8</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>8</v>
-      </c>
-      <c r="J23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23">
-        <v>33.3</v>
-      </c>
-      <c r="M23" s="1">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23">
-        <v>0.38</v>
-      </c>
-      <c r="Q23" s="1">
-        <v>8</v>
-      </c>
-      <c r="R23" t="s">
-        <v>11</v>
-      </c>
-      <c r="S23">
-        <v>5.7</v>
-      </c>
-      <c r="T23">
-        <v>7.7</v>
-      </c>
-      <c r="U23">
-        <v>15</v>
-      </c>
-      <c r="W23" s="1">
-        <v>8</v>
-      </c>
-      <c r="X23" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y23">
-        <v>17</v>
-      </c>
-      <c r="Z23">
-        <v>23</v>
-      </c>
-      <c r="AA23">
-        <v>45</v>
-      </c>
-      <c r="AB23">
-        <v>-28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>